<commit_message>
first pass at pathogen mapping and host-pathogen associations
</commit_message>
<xml_diff>
--- a/data/raw_data/2023-01-06_data.xlsx
+++ b/data/raw_data/2023-01-06_data.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="rodent" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="pathogen" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="pathogen_sequences" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="known_zoonoses" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5556" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5635" uniqueCount="308">
   <si>
     <t>study_id</t>
   </si>
@@ -796,6 +797,9 @@
     <t>AJ269554</t>
   </si>
   <si>
+    <t>Urotrichis</t>
+  </si>
+  <si>
     <t>EU929070</t>
   </si>
   <si>
@@ -867,6 +871,75 @@
   <si>
     <t>MW039391</t>
   </si>
+  <si>
+    <t>pathogen_id</t>
+  </si>
+  <si>
+    <t>known_zoonosis</t>
+  </si>
+  <si>
+    <t>disease_name</t>
+  </si>
+  <si>
+    <t>icd_10</t>
+  </si>
+  <si>
+    <t>disease_reference</t>
+  </si>
+  <si>
+    <t>Hantavirus Cardio-Pulmonary Syndrome</t>
+  </si>
+  <si>
+    <t>B33.4</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1126/science.8235615</t>
+  </si>
+  <si>
+    <t>Hemorrhagic Fever with Renal Syndrome</t>
+  </si>
+  <si>
+    <t>A98.5</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1086/515185</t>
+  </si>
+  <si>
+    <t>Lymphocytic Choriomeningitis, Congenital Lymphocytic Choriomeningitis</t>
+  </si>
+  <si>
+    <t>A87.2</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/cid/article/33/3/370/278006</t>
+  </si>
+  <si>
+    <t>Nephropathia Epidemica</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/oxfordjournals.qjmed.a068385</t>
+  </si>
+  <si>
+    <t>Saaremaa virus</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3201%2Feid1404.071310</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.7326/0003-4819-113-5-385</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1159/000188762</t>
+  </si>
+  <si>
+    <t>Lassa Fever</t>
+  </si>
+  <si>
+    <t>A96.2</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.4269/ajtmh.1970.19.670</t>
+  </si>
 </sst>
 </file>
 
@@ -875,7 +948,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -918,6 +991,10 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -939,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -979,6 +1056,21 @@
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1000,6 +1092,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -30791,8 +30887,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.13"/>
-    <col customWidth="1" min="3" max="3" width="14.5"/>
-    <col customWidth="1" min="4" max="4" width="26.5"/>
+    <col customWidth="1" min="3" max="4" width="14.5"/>
+    <col customWidth="1" min="5" max="5" width="26.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -30803,12 +30899,15 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>253</v>
       </c>
     </row>
@@ -30820,12 +30919,15 @@
         <v>3.0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>254</v>
       </c>
     </row>
@@ -30837,12 +30939,15 @@
         <v>3.0</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>255</v>
       </c>
     </row>
@@ -30854,12 +30959,15 @@
         <v>3.0</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>256</v>
       </c>
     </row>
@@ -30871,12 +30979,15 @@
         <v>3.0</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>257</v>
       </c>
     </row>
@@ -30888,12 +30999,15 @@
         <v>3.0</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>258</v>
       </c>
     </row>
@@ -30905,12 +31019,15 @@
         <v>3.0</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>259</v>
       </c>
     </row>
@@ -30922,13 +31039,16 @@
         <v>6.0</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>260</v>
+      <c r="F8" s="12" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="9">
@@ -30939,13 +31059,16 @@
         <v>6.0</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>261</v>
+      <c r="F9" s="9" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="10">
@@ -30956,13 +31079,16 @@
         <v>6.0</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>262</v>
+      <c r="F10" s="9" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="11">
@@ -30973,13 +31099,16 @@
         <v>6.0</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>263</v>
+      <c r="F11" s="12" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="12">
@@ -30990,13 +31119,16 @@
         <v>6.0</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>264</v>
+      <c r="F12" s="9" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="13">
@@ -31007,13 +31139,16 @@
         <v>6.0</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>265</v>
+      <c r="F13" s="9" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="14">
@@ -31024,13 +31159,16 @@
         <v>6.0</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>266</v>
+      <c r="F14" s="12" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="15">
@@ -31041,13 +31179,16 @@
         <v>6.0</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>267</v>
+      <c r="F15" s="9" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="16">
@@ -31058,13 +31199,16 @@
         <v>6.0</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>268</v>
+      <c r="F16" s="9" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="17">
@@ -31075,13 +31219,16 @@
         <v>7.0</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>269</v>
+      <c r="F17" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="18">
@@ -31092,13 +31239,16 @@
         <v>7.0</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>270</v>
+      <c r="F18" s="1" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="19">
@@ -31109,13 +31259,16 @@
         <v>7.0</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>271</v>
+      <c r="F19" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="20">
@@ -31126,13 +31279,16 @@
         <v>7.0</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>272</v>
+      <c r="F20" s="1" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="21">
@@ -31143,13 +31299,16 @@
         <v>7.0</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>273</v>
+      <c r="F21" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="22">
@@ -31160,13 +31319,16 @@
         <v>7.0</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>274</v>
+      <c r="F22" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="23">
@@ -31177,13 +31339,16 @@
         <v>7.0</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>275</v>
+      <c r="F23" s="1" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="24">
@@ -31194,13 +31359,16 @@
         <v>7.0</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>276</v>
+      <c r="F24" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="25">
@@ -31211,13 +31379,16 @@
         <v>7.0</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>277</v>
+      <c r="F25" s="1" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="26">
@@ -31228,13 +31399,16 @@
         <v>7.0</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>278</v>
+      <c r="F26" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="27">
@@ -31245,13 +31419,16 @@
         <v>7.0</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>279</v>
+      <c r="F27" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="28">
@@ -31262,13 +31439,16 @@
         <v>9.0</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>280</v>
+      <c r="F28" s="1" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="29">
@@ -31279,13 +31459,16 @@
         <v>9.0</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>281</v>
+      <c r="F29" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="30">
@@ -31296,13 +31479,16 @@
         <v>9.0</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>282</v>
+      <c r="F30" s="1" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="31">
@@ -31313,16 +31499,3612 @@
         <v>9.0</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>283</v>
+      <c r="F31" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="26.63"/>
+    <col customWidth="1" min="4" max="4" width="13.38"/>
+    <col customWidth="1" min="5" max="5" width="30.13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="15">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="D6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="16">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="15">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="16">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="15">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="14"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="14"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="14"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="14"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="14"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="14"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="14"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="14"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="14"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="14"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="14"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="14"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="14"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="14"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="14"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="14"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="14"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="14"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="14"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="14"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="14"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="14"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="14"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="14"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="14"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="14"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="14"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="14"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="14"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="14"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="14"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="14"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="14"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="14"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="14"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="14"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="14"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="14"/>
+      <c r="B105" s="14"/>
+      <c r="C105" s="14"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="14"/>
+      <c r="B106" s="14"/>
+      <c r="C106" s="14"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="14"/>
+      <c r="B107" s="14"/>
+      <c r="C107" s="14"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="14"/>
+      <c r="B108" s="14"/>
+      <c r="C108" s="14"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="14"/>
+      <c r="B109" s="14"/>
+      <c r="C109" s="14"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="14"/>
+      <c r="B110" s="14"/>
+      <c r="C110" s="14"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="14"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="14"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="14"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="14"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="14"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="14"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="14"/>
+      <c r="B114" s="14"/>
+      <c r="C114" s="14"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="14"/>
+      <c r="B115" s="14"/>
+      <c r="C115" s="14"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="14"/>
+      <c r="B116" s="14"/>
+      <c r="C116" s="14"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="14"/>
+      <c r="B117" s="14"/>
+      <c r="C117" s="14"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="14"/>
+      <c r="B118" s="14"/>
+      <c r="C118" s="14"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="14"/>
+      <c r="B119" s="14"/>
+      <c r="C119" s="14"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="14"/>
+      <c r="B120" s="14"/>
+      <c r="C120" s="14"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="14"/>
+      <c r="B121" s="14"/>
+      <c r="C121" s="14"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="14"/>
+      <c r="B122" s="14"/>
+      <c r="C122" s="14"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="14"/>
+      <c r="B123" s="14"/>
+      <c r="C123" s="14"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="14"/>
+      <c r="B124" s="14"/>
+      <c r="C124" s="14"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="14"/>
+      <c r="B125" s="14"/>
+      <c r="C125" s="14"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="14"/>
+      <c r="B126" s="14"/>
+      <c r="C126" s="14"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="14"/>
+      <c r="B127" s="14"/>
+      <c r="C127" s="14"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="14"/>
+      <c r="B128" s="14"/>
+      <c r="C128" s="14"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="14"/>
+      <c r="B129" s="14"/>
+      <c r="C129" s="14"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="14"/>
+      <c r="B130" s="14"/>
+      <c r="C130" s="14"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="14"/>
+      <c r="B131" s="14"/>
+      <c r="C131" s="14"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="14"/>
+      <c r="B132" s="14"/>
+      <c r="C132" s="14"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="14"/>
+      <c r="B133" s="14"/>
+      <c r="C133" s="14"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="14"/>
+      <c r="B134" s="14"/>
+      <c r="C134" s="14"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="14"/>
+      <c r="B135" s="14"/>
+      <c r="C135" s="14"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="14"/>
+      <c r="B136" s="14"/>
+      <c r="C136" s="14"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="14"/>
+      <c r="B137" s="14"/>
+      <c r="C137" s="14"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="14"/>
+      <c r="B138" s="14"/>
+      <c r="C138" s="14"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="14"/>
+      <c r="B139" s="14"/>
+      <c r="C139" s="14"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="14"/>
+      <c r="B140" s="14"/>
+      <c r="C140" s="14"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="14"/>
+      <c r="B141" s="14"/>
+      <c r="C141" s="14"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="14"/>
+      <c r="B142" s="14"/>
+      <c r="C142" s="14"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="14"/>
+      <c r="B143" s="14"/>
+      <c r="C143" s="14"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="14"/>
+      <c r="B144" s="14"/>
+      <c r="C144" s="14"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="14"/>
+      <c r="B145" s="14"/>
+      <c r="C145" s="14"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="14"/>
+      <c r="B146" s="14"/>
+      <c r="C146" s="14"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="14"/>
+      <c r="B147" s="14"/>
+      <c r="C147" s="14"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="14"/>
+      <c r="B148" s="14"/>
+      <c r="C148" s="14"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="14"/>
+      <c r="B149" s="14"/>
+      <c r="C149" s="14"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="14"/>
+      <c r="B150" s="14"/>
+      <c r="C150" s="14"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="14"/>
+      <c r="B151" s="14"/>
+      <c r="C151" s="14"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="14"/>
+      <c r="B152" s="14"/>
+      <c r="C152" s="14"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="14"/>
+      <c r="B153" s="14"/>
+      <c r="C153" s="14"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="14"/>
+      <c r="B154" s="14"/>
+      <c r="C154" s="14"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="14"/>
+      <c r="B155" s="14"/>
+      <c r="C155" s="14"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="14"/>
+      <c r="B156" s="14"/>
+      <c r="C156" s="14"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="14"/>
+      <c r="B157" s="14"/>
+      <c r="C157" s="14"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="14"/>
+      <c r="B158" s="14"/>
+      <c r="C158" s="14"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="14"/>
+      <c r="B159" s="14"/>
+      <c r="C159" s="14"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="14"/>
+      <c r="B160" s="14"/>
+      <c r="C160" s="14"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="14"/>
+      <c r="B161" s="14"/>
+      <c r="C161" s="14"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="14"/>
+      <c r="B162" s="14"/>
+      <c r="C162" s="14"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="14"/>
+      <c r="B163" s="14"/>
+      <c r="C163" s="14"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="14"/>
+      <c r="B164" s="14"/>
+      <c r="C164" s="14"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="14"/>
+      <c r="B165" s="14"/>
+      <c r="C165" s="14"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="14"/>
+      <c r="B166" s="14"/>
+      <c r="C166" s="14"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="14"/>
+      <c r="B167" s="14"/>
+      <c r="C167" s="14"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="14"/>
+      <c r="B168" s="14"/>
+      <c r="C168" s="14"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="14"/>
+      <c r="B169" s="14"/>
+      <c r="C169" s="14"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="14"/>
+      <c r="B170" s="14"/>
+      <c r="C170" s="14"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="14"/>
+      <c r="B171" s="14"/>
+      <c r="C171" s="14"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="14"/>
+      <c r="B172" s="14"/>
+      <c r="C172" s="14"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="14"/>
+      <c r="B173" s="14"/>
+      <c r="C173" s="14"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="14"/>
+      <c r="B174" s="14"/>
+      <c r="C174" s="14"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="14"/>
+      <c r="B175" s="14"/>
+      <c r="C175" s="14"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="14"/>
+      <c r="B176" s="14"/>
+      <c r="C176" s="14"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="14"/>
+      <c r="B177" s="14"/>
+      <c r="C177" s="14"/>
+    </row>
+    <row r="178">
+      <c r="A178" s="14"/>
+      <c r="B178" s="14"/>
+      <c r="C178" s="14"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="14"/>
+      <c r="B179" s="14"/>
+      <c r="C179" s="14"/>
+    </row>
+    <row r="180">
+      <c r="A180" s="14"/>
+      <c r="B180" s="14"/>
+      <c r="C180" s="14"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="14"/>
+      <c r="B181" s="14"/>
+      <c r="C181" s="14"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="14"/>
+      <c r="B182" s="14"/>
+      <c r="C182" s="14"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="14"/>
+      <c r="B183" s="14"/>
+      <c r="C183" s="14"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="14"/>
+      <c r="B184" s="14"/>
+      <c r="C184" s="14"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="14"/>
+      <c r="B185" s="14"/>
+      <c r="C185" s="14"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="14"/>
+      <c r="B186" s="14"/>
+      <c r="C186" s="14"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="14"/>
+      <c r="B187" s="14"/>
+      <c r="C187" s="14"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="14"/>
+      <c r="B188" s="14"/>
+      <c r="C188" s="14"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="14"/>
+      <c r="B189" s="14"/>
+      <c r="C189" s="14"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="14"/>
+      <c r="B190" s="14"/>
+      <c r="C190" s="14"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="14"/>
+      <c r="B191" s="14"/>
+      <c r="C191" s="14"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="14"/>
+      <c r="B192" s="14"/>
+      <c r="C192" s="14"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="14"/>
+      <c r="B193" s="14"/>
+      <c r="C193" s="14"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="14"/>
+      <c r="B194" s="14"/>
+      <c r="C194" s="14"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="14"/>
+      <c r="B195" s="14"/>
+      <c r="C195" s="14"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="14"/>
+      <c r="B196" s="14"/>
+      <c r="C196" s="14"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="14"/>
+      <c r="B197" s="14"/>
+      <c r="C197" s="14"/>
+    </row>
+    <row r="198">
+      <c r="A198" s="14"/>
+      <c r="B198" s="14"/>
+      <c r="C198" s="14"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="14"/>
+      <c r="B199" s="14"/>
+      <c r="C199" s="14"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="14"/>
+      <c r="B200" s="14"/>
+      <c r="C200" s="14"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="14"/>
+      <c r="B201" s="14"/>
+      <c r="C201" s="14"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="14"/>
+      <c r="B202" s="14"/>
+      <c r="C202" s="14"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="14"/>
+      <c r="B203" s="14"/>
+      <c r="C203" s="14"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="14"/>
+      <c r="B204" s="14"/>
+      <c r="C204" s="14"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="14"/>
+      <c r="B205" s="14"/>
+      <c r="C205" s="14"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="14"/>
+      <c r="B206" s="14"/>
+      <c r="C206" s="14"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="14"/>
+      <c r="B207" s="14"/>
+      <c r="C207" s="14"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="14"/>
+      <c r="B208" s="14"/>
+      <c r="C208" s="14"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="14"/>
+      <c r="B209" s="14"/>
+      <c r="C209" s="14"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="14"/>
+      <c r="B210" s="14"/>
+      <c r="C210" s="14"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="14"/>
+      <c r="B211" s="14"/>
+      <c r="C211" s="14"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="14"/>
+      <c r="B212" s="14"/>
+      <c r="C212" s="14"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="14"/>
+      <c r="B213" s="14"/>
+      <c r="C213" s="14"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="14"/>
+      <c r="B214" s="14"/>
+      <c r="C214" s="14"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="14"/>
+      <c r="B215" s="14"/>
+      <c r="C215" s="14"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="14"/>
+      <c r="B216" s="14"/>
+      <c r="C216" s="14"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="14"/>
+      <c r="B217" s="14"/>
+      <c r="C217" s="14"/>
+    </row>
+    <row r="218">
+      <c r="A218" s="14"/>
+      <c r="B218" s="14"/>
+      <c r="C218" s="14"/>
+    </row>
+    <row r="219">
+      <c r="A219" s="14"/>
+      <c r="B219" s="14"/>
+      <c r="C219" s="14"/>
+    </row>
+    <row r="220">
+      <c r="A220" s="14"/>
+      <c r="B220" s="14"/>
+      <c r="C220" s="14"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="14"/>
+      <c r="B221" s="14"/>
+      <c r="C221" s="14"/>
+    </row>
+    <row r="222">
+      <c r="A222" s="14"/>
+      <c r="B222" s="14"/>
+      <c r="C222" s="14"/>
+    </row>
+    <row r="223">
+      <c r="A223" s="14"/>
+      <c r="B223" s="14"/>
+      <c r="C223" s="14"/>
+    </row>
+    <row r="224">
+      <c r="A224" s="14"/>
+      <c r="B224" s="14"/>
+      <c r="C224" s="14"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="14"/>
+      <c r="B225" s="14"/>
+      <c r="C225" s="14"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="14"/>
+      <c r="B226" s="14"/>
+      <c r="C226" s="14"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="14"/>
+      <c r="B227" s="14"/>
+      <c r="C227" s="14"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="14"/>
+      <c r="B228" s="14"/>
+      <c r="C228" s="14"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="14"/>
+      <c r="B229" s="14"/>
+      <c r="C229" s="14"/>
+    </row>
+    <row r="230">
+      <c r="A230" s="14"/>
+      <c r="B230" s="14"/>
+      <c r="C230" s="14"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="14"/>
+      <c r="B231" s="14"/>
+      <c r="C231" s="14"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="14"/>
+      <c r="B232" s="14"/>
+      <c r="C232" s="14"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="14"/>
+      <c r="B233" s="14"/>
+      <c r="C233" s="14"/>
+    </row>
+    <row r="234">
+      <c r="A234" s="14"/>
+      <c r="B234" s="14"/>
+      <c r="C234" s="14"/>
+    </row>
+    <row r="235">
+      <c r="A235" s="14"/>
+      <c r="B235" s="14"/>
+      <c r="C235" s="14"/>
+    </row>
+    <row r="236">
+      <c r="A236" s="14"/>
+      <c r="B236" s="14"/>
+      <c r="C236" s="14"/>
+    </row>
+    <row r="237">
+      <c r="A237" s="14"/>
+      <c r="B237" s="14"/>
+      <c r="C237" s="14"/>
+    </row>
+    <row r="238">
+      <c r="A238" s="14"/>
+      <c r="B238" s="14"/>
+      <c r="C238" s="14"/>
+    </row>
+    <row r="239">
+      <c r="A239" s="14"/>
+      <c r="B239" s="14"/>
+      <c r="C239" s="14"/>
+    </row>
+    <row r="240">
+      <c r="A240" s="14"/>
+      <c r="B240" s="14"/>
+      <c r="C240" s="14"/>
+    </row>
+    <row r="241">
+      <c r="A241" s="14"/>
+      <c r="B241" s="14"/>
+      <c r="C241" s="14"/>
+    </row>
+    <row r="242">
+      <c r="A242" s="14"/>
+      <c r="B242" s="14"/>
+      <c r="C242" s="14"/>
+    </row>
+    <row r="243">
+      <c r="A243" s="14"/>
+      <c r="B243" s="14"/>
+      <c r="C243" s="14"/>
+    </row>
+    <row r="244">
+      <c r="A244" s="14"/>
+      <c r="B244" s="14"/>
+      <c r="C244" s="14"/>
+    </row>
+    <row r="245">
+      <c r="A245" s="14"/>
+      <c r="B245" s="14"/>
+      <c r="C245" s="14"/>
+    </row>
+    <row r="246">
+      <c r="A246" s="14"/>
+      <c r="B246" s="14"/>
+      <c r="C246" s="14"/>
+    </row>
+    <row r="247">
+      <c r="A247" s="14"/>
+      <c r="B247" s="14"/>
+      <c r="C247" s="14"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="14"/>
+      <c r="B248" s="14"/>
+      <c r="C248" s="14"/>
+    </row>
+    <row r="249">
+      <c r="A249" s="14"/>
+      <c r="B249" s="14"/>
+      <c r="C249" s="14"/>
+    </row>
+    <row r="250">
+      <c r="A250" s="14"/>
+      <c r="B250" s="14"/>
+      <c r="C250" s="14"/>
+    </row>
+    <row r="251">
+      <c r="A251" s="14"/>
+      <c r="B251" s="14"/>
+      <c r="C251" s="14"/>
+    </row>
+    <row r="252">
+      <c r="A252" s="14"/>
+      <c r="B252" s="14"/>
+      <c r="C252" s="14"/>
+    </row>
+    <row r="253">
+      <c r="A253" s="14"/>
+      <c r="B253" s="14"/>
+      <c r="C253" s="14"/>
+    </row>
+    <row r="254">
+      <c r="A254" s="14"/>
+      <c r="B254" s="14"/>
+      <c r="C254" s="14"/>
+    </row>
+    <row r="255">
+      <c r="A255" s="14"/>
+      <c r="B255" s="14"/>
+      <c r="C255" s="14"/>
+    </row>
+    <row r="256">
+      <c r="A256" s="14"/>
+      <c r="B256" s="14"/>
+      <c r="C256" s="14"/>
+    </row>
+    <row r="257">
+      <c r="A257" s="14"/>
+      <c r="B257" s="14"/>
+      <c r="C257" s="14"/>
+    </row>
+    <row r="258">
+      <c r="A258" s="14"/>
+      <c r="B258" s="14"/>
+      <c r="C258" s="14"/>
+    </row>
+    <row r="259">
+      <c r="A259" s="14"/>
+      <c r="B259" s="14"/>
+      <c r="C259" s="14"/>
+    </row>
+    <row r="260">
+      <c r="A260" s="14"/>
+      <c r="B260" s="14"/>
+      <c r="C260" s="14"/>
+    </row>
+    <row r="261">
+      <c r="A261" s="14"/>
+      <c r="B261" s="14"/>
+      <c r="C261" s="14"/>
+    </row>
+    <row r="262">
+      <c r="A262" s="14"/>
+      <c r="B262" s="14"/>
+      <c r="C262" s="14"/>
+    </row>
+    <row r="263">
+      <c r="A263" s="14"/>
+      <c r="B263" s="14"/>
+      <c r="C263" s="14"/>
+    </row>
+    <row r="264">
+      <c r="A264" s="14"/>
+      <c r="B264" s="14"/>
+      <c r="C264" s="14"/>
+    </row>
+    <row r="265">
+      <c r="A265" s="14"/>
+      <c r="B265" s="14"/>
+      <c r="C265" s="14"/>
+    </row>
+    <row r="266">
+      <c r="A266" s="14"/>
+      <c r="B266" s="14"/>
+      <c r="C266" s="14"/>
+    </row>
+    <row r="267">
+      <c r="A267" s="14"/>
+      <c r="B267" s="14"/>
+      <c r="C267" s="14"/>
+    </row>
+    <row r="268">
+      <c r="A268" s="14"/>
+      <c r="B268" s="14"/>
+      <c r="C268" s="14"/>
+    </row>
+    <row r="269">
+      <c r="A269" s="14"/>
+      <c r="B269" s="14"/>
+      <c r="C269" s="14"/>
+    </row>
+    <row r="270">
+      <c r="A270" s="14"/>
+      <c r="B270" s="14"/>
+      <c r="C270" s="14"/>
+    </row>
+    <row r="271">
+      <c r="A271" s="14"/>
+      <c r="B271" s="14"/>
+      <c r="C271" s="14"/>
+    </row>
+    <row r="272">
+      <c r="A272" s="14"/>
+      <c r="B272" s="14"/>
+      <c r="C272" s="14"/>
+    </row>
+    <row r="273">
+      <c r="A273" s="14"/>
+      <c r="B273" s="14"/>
+      <c r="C273" s="14"/>
+    </row>
+    <row r="274">
+      <c r="A274" s="14"/>
+      <c r="B274" s="14"/>
+      <c r="C274" s="14"/>
+    </row>
+    <row r="275">
+      <c r="A275" s="14"/>
+      <c r="B275" s="14"/>
+      <c r="C275" s="14"/>
+    </row>
+    <row r="276">
+      <c r="A276" s="14"/>
+      <c r="B276" s="14"/>
+      <c r="C276" s="14"/>
+    </row>
+    <row r="277">
+      <c r="A277" s="14"/>
+      <c r="B277" s="14"/>
+      <c r="C277" s="14"/>
+    </row>
+    <row r="278">
+      <c r="A278" s="14"/>
+      <c r="B278" s="14"/>
+      <c r="C278" s="14"/>
+    </row>
+    <row r="279">
+      <c r="A279" s="14"/>
+      <c r="B279" s="14"/>
+      <c r="C279" s="14"/>
+    </row>
+    <row r="280">
+      <c r="A280" s="14"/>
+      <c r="B280" s="14"/>
+      <c r="C280" s="14"/>
+    </row>
+    <row r="281">
+      <c r="A281" s="14"/>
+      <c r="B281" s="14"/>
+      <c r="C281" s="14"/>
+    </row>
+    <row r="282">
+      <c r="A282" s="14"/>
+      <c r="B282" s="14"/>
+      <c r="C282" s="14"/>
+    </row>
+    <row r="283">
+      <c r="A283" s="14"/>
+      <c r="B283" s="14"/>
+      <c r="C283" s="14"/>
+    </row>
+    <row r="284">
+      <c r="A284" s="14"/>
+      <c r="B284" s="14"/>
+      <c r="C284" s="14"/>
+    </row>
+    <row r="285">
+      <c r="A285" s="14"/>
+      <c r="B285" s="14"/>
+      <c r="C285" s="14"/>
+    </row>
+    <row r="286">
+      <c r="A286" s="14"/>
+      <c r="B286" s="14"/>
+      <c r="C286" s="14"/>
+    </row>
+    <row r="287">
+      <c r="A287" s="14"/>
+      <c r="B287" s="14"/>
+      <c r="C287" s="14"/>
+    </row>
+    <row r="288">
+      <c r="A288" s="14"/>
+      <c r="B288" s="14"/>
+      <c r="C288" s="14"/>
+    </row>
+    <row r="289">
+      <c r="A289" s="14"/>
+      <c r="B289" s="14"/>
+      <c r="C289" s="14"/>
+    </row>
+    <row r="290">
+      <c r="A290" s="14"/>
+      <c r="B290" s="14"/>
+      <c r="C290" s="14"/>
+    </row>
+    <row r="291">
+      <c r="A291" s="14"/>
+      <c r="B291" s="14"/>
+      <c r="C291" s="14"/>
+    </row>
+    <row r="292">
+      <c r="A292" s="14"/>
+      <c r="B292" s="14"/>
+      <c r="C292" s="14"/>
+    </row>
+    <row r="293">
+      <c r="A293" s="14"/>
+      <c r="B293" s="14"/>
+      <c r="C293" s="14"/>
+    </row>
+    <row r="294">
+      <c r="A294" s="14"/>
+      <c r="B294" s="14"/>
+      <c r="C294" s="14"/>
+    </row>
+    <row r="295">
+      <c r="A295" s="14"/>
+      <c r="B295" s="14"/>
+      <c r="C295" s="14"/>
+    </row>
+    <row r="296">
+      <c r="A296" s="14"/>
+      <c r="B296" s="14"/>
+      <c r="C296" s="14"/>
+    </row>
+    <row r="297">
+      <c r="A297" s="14"/>
+      <c r="B297" s="14"/>
+      <c r="C297" s="14"/>
+    </row>
+    <row r="298">
+      <c r="A298" s="14"/>
+      <c r="B298" s="14"/>
+      <c r="C298" s="14"/>
+    </row>
+    <row r="299">
+      <c r="A299" s="14"/>
+      <c r="B299" s="14"/>
+      <c r="C299" s="14"/>
+    </row>
+    <row r="300">
+      <c r="A300" s="14"/>
+      <c r="B300" s="14"/>
+      <c r="C300" s="14"/>
+    </row>
+    <row r="301">
+      <c r="A301" s="14"/>
+      <c r="B301" s="14"/>
+      <c r="C301" s="14"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="14"/>
+      <c r="B302" s="14"/>
+      <c r="C302" s="14"/>
+    </row>
+    <row r="303">
+      <c r="A303" s="14"/>
+      <c r="B303" s="14"/>
+      <c r="C303" s="14"/>
+    </row>
+    <row r="304">
+      <c r="A304" s="14"/>
+      <c r="B304" s="14"/>
+      <c r="C304" s="14"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="14"/>
+      <c r="B305" s="14"/>
+      <c r="C305" s="14"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="14"/>
+      <c r="B306" s="14"/>
+      <c r="C306" s="14"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="14"/>
+      <c r="B307" s="14"/>
+      <c r="C307" s="14"/>
+    </row>
+    <row r="308">
+      <c r="A308" s="14"/>
+      <c r="B308" s="14"/>
+      <c r="C308" s="14"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="14"/>
+      <c r="B309" s="14"/>
+      <c r="C309" s="14"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="14"/>
+      <c r="B310" s="14"/>
+      <c r="C310" s="14"/>
+    </row>
+    <row r="311">
+      <c r="A311" s="14"/>
+      <c r="B311" s="14"/>
+      <c r="C311" s="14"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="14"/>
+      <c r="B312" s="14"/>
+      <c r="C312" s="14"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="14"/>
+      <c r="B313" s="14"/>
+      <c r="C313" s="14"/>
+    </row>
+    <row r="314">
+      <c r="A314" s="14"/>
+      <c r="B314" s="14"/>
+      <c r="C314" s="14"/>
+    </row>
+    <row r="315">
+      <c r="A315" s="14"/>
+      <c r="B315" s="14"/>
+      <c r="C315" s="14"/>
+    </row>
+    <row r="316">
+      <c r="A316" s="14"/>
+      <c r="B316" s="14"/>
+      <c r="C316" s="14"/>
+    </row>
+    <row r="317">
+      <c r="A317" s="14"/>
+      <c r="B317" s="14"/>
+      <c r="C317" s="14"/>
+    </row>
+    <row r="318">
+      <c r="A318" s="14"/>
+      <c r="B318" s="14"/>
+      <c r="C318" s="14"/>
+    </row>
+    <row r="319">
+      <c r="A319" s="14"/>
+      <c r="B319" s="14"/>
+      <c r="C319" s="14"/>
+    </row>
+    <row r="320">
+      <c r="A320" s="14"/>
+      <c r="B320" s="14"/>
+      <c r="C320" s="14"/>
+    </row>
+    <row r="321">
+      <c r="A321" s="14"/>
+      <c r="B321" s="14"/>
+      <c r="C321" s="14"/>
+    </row>
+    <row r="322">
+      <c r="A322" s="14"/>
+      <c r="B322" s="14"/>
+      <c r="C322" s="14"/>
+    </row>
+    <row r="323">
+      <c r="A323" s="14"/>
+      <c r="B323" s="14"/>
+      <c r="C323" s="14"/>
+    </row>
+    <row r="324">
+      <c r="A324" s="14"/>
+      <c r="B324" s="14"/>
+      <c r="C324" s="14"/>
+    </row>
+    <row r="325">
+      <c r="A325" s="14"/>
+      <c r="B325" s="14"/>
+      <c r="C325" s="14"/>
+    </row>
+    <row r="326">
+      <c r="A326" s="14"/>
+      <c r="B326" s="14"/>
+      <c r="C326" s="14"/>
+    </row>
+    <row r="327">
+      <c r="A327" s="14"/>
+      <c r="B327" s="14"/>
+      <c r="C327" s="14"/>
+    </row>
+    <row r="328">
+      <c r="A328" s="14"/>
+      <c r="B328" s="14"/>
+      <c r="C328" s="14"/>
+    </row>
+    <row r="329">
+      <c r="A329" s="14"/>
+      <c r="B329" s="14"/>
+      <c r="C329" s="14"/>
+    </row>
+    <row r="330">
+      <c r="A330" s="14"/>
+      <c r="B330" s="14"/>
+      <c r="C330" s="14"/>
+    </row>
+    <row r="331">
+      <c r="A331" s="14"/>
+      <c r="B331" s="14"/>
+      <c r="C331" s="14"/>
+    </row>
+    <row r="332">
+      <c r="A332" s="14"/>
+      <c r="B332" s="14"/>
+      <c r="C332" s="14"/>
+    </row>
+    <row r="333">
+      <c r="A333" s="14"/>
+      <c r="B333" s="14"/>
+      <c r="C333" s="14"/>
+    </row>
+    <row r="334">
+      <c r="A334" s="14"/>
+      <c r="B334" s="14"/>
+      <c r="C334" s="14"/>
+    </row>
+    <row r="335">
+      <c r="A335" s="14"/>
+      <c r="B335" s="14"/>
+      <c r="C335" s="14"/>
+    </row>
+    <row r="336">
+      <c r="A336" s="14"/>
+      <c r="B336" s="14"/>
+      <c r="C336" s="14"/>
+    </row>
+    <row r="337">
+      <c r="A337" s="14"/>
+      <c r="B337" s="14"/>
+      <c r="C337" s="14"/>
+    </row>
+    <row r="338">
+      <c r="A338" s="14"/>
+      <c r="B338" s="14"/>
+      <c r="C338" s="14"/>
+    </row>
+    <row r="339">
+      <c r="A339" s="14"/>
+      <c r="B339" s="14"/>
+      <c r="C339" s="14"/>
+    </row>
+    <row r="340">
+      <c r="A340" s="14"/>
+      <c r="B340" s="14"/>
+      <c r="C340" s="14"/>
+    </row>
+    <row r="341">
+      <c r="A341" s="14"/>
+      <c r="B341" s="14"/>
+      <c r="C341" s="14"/>
+    </row>
+    <row r="342">
+      <c r="A342" s="14"/>
+      <c r="B342" s="14"/>
+      <c r="C342" s="14"/>
+    </row>
+    <row r="343">
+      <c r="A343" s="14"/>
+      <c r="B343" s="14"/>
+      <c r="C343" s="14"/>
+    </row>
+    <row r="344">
+      <c r="A344" s="14"/>
+      <c r="B344" s="14"/>
+      <c r="C344" s="14"/>
+    </row>
+    <row r="345">
+      <c r="A345" s="14"/>
+      <c r="B345" s="14"/>
+      <c r="C345" s="14"/>
+    </row>
+    <row r="346">
+      <c r="A346" s="14"/>
+      <c r="B346" s="14"/>
+      <c r="C346" s="14"/>
+    </row>
+    <row r="347">
+      <c r="A347" s="14"/>
+      <c r="B347" s="14"/>
+      <c r="C347" s="14"/>
+    </row>
+    <row r="348">
+      <c r="A348" s="14"/>
+      <c r="B348" s="14"/>
+      <c r="C348" s="14"/>
+    </row>
+    <row r="349">
+      <c r="A349" s="14"/>
+      <c r="B349" s="14"/>
+      <c r="C349" s="14"/>
+    </row>
+    <row r="350">
+      <c r="A350" s="14"/>
+      <c r="B350" s="14"/>
+      <c r="C350" s="14"/>
+    </row>
+    <row r="351">
+      <c r="A351" s="14"/>
+      <c r="B351" s="14"/>
+      <c r="C351" s="14"/>
+    </row>
+    <row r="352">
+      <c r="A352" s="14"/>
+      <c r="B352" s="14"/>
+      <c r="C352" s="14"/>
+    </row>
+    <row r="353">
+      <c r="A353" s="14"/>
+      <c r="B353" s="14"/>
+      <c r="C353" s="14"/>
+    </row>
+    <row r="354">
+      <c r="A354" s="14"/>
+      <c r="B354" s="14"/>
+      <c r="C354" s="14"/>
+    </row>
+    <row r="355">
+      <c r="A355" s="14"/>
+      <c r="B355" s="14"/>
+      <c r="C355" s="14"/>
+    </row>
+    <row r="356">
+      <c r="A356" s="14"/>
+      <c r="B356" s="14"/>
+      <c r="C356" s="14"/>
+    </row>
+    <row r="357">
+      <c r="A357" s="14"/>
+      <c r="B357" s="14"/>
+      <c r="C357" s="14"/>
+    </row>
+    <row r="358">
+      <c r="A358" s="14"/>
+      <c r="B358" s="14"/>
+      <c r="C358" s="14"/>
+    </row>
+    <row r="359">
+      <c r="A359" s="14"/>
+      <c r="B359" s="14"/>
+      <c r="C359" s="14"/>
+    </row>
+    <row r="360">
+      <c r="A360" s="14"/>
+      <c r="B360" s="14"/>
+      <c r="C360" s="14"/>
+    </row>
+    <row r="361">
+      <c r="A361" s="14"/>
+      <c r="B361" s="14"/>
+      <c r="C361" s="14"/>
+    </row>
+    <row r="362">
+      <c r="A362" s="14"/>
+      <c r="B362" s="14"/>
+      <c r="C362" s="14"/>
+    </row>
+    <row r="363">
+      <c r="A363" s="14"/>
+      <c r="B363" s="14"/>
+      <c r="C363" s="14"/>
+    </row>
+    <row r="364">
+      <c r="A364" s="14"/>
+      <c r="B364" s="14"/>
+      <c r="C364" s="14"/>
+    </row>
+    <row r="365">
+      <c r="A365" s="14"/>
+      <c r="B365" s="14"/>
+      <c r="C365" s="14"/>
+    </row>
+    <row r="366">
+      <c r="A366" s="14"/>
+      <c r="B366" s="14"/>
+      <c r="C366" s="14"/>
+    </row>
+    <row r="367">
+      <c r="A367" s="14"/>
+      <c r="B367" s="14"/>
+      <c r="C367" s="14"/>
+    </row>
+    <row r="368">
+      <c r="A368" s="14"/>
+      <c r="B368" s="14"/>
+      <c r="C368" s="14"/>
+    </row>
+    <row r="369">
+      <c r="A369" s="14"/>
+      <c r="B369" s="14"/>
+      <c r="C369" s="14"/>
+    </row>
+    <row r="370">
+      <c r="A370" s="14"/>
+      <c r="B370" s="14"/>
+      <c r="C370" s="14"/>
+    </row>
+    <row r="371">
+      <c r="A371" s="14"/>
+      <c r="B371" s="14"/>
+      <c r="C371" s="14"/>
+    </row>
+    <row r="372">
+      <c r="A372" s="14"/>
+      <c r="B372" s="14"/>
+      <c r="C372" s="14"/>
+    </row>
+    <row r="373">
+      <c r="A373" s="14"/>
+      <c r="B373" s="14"/>
+      <c r="C373" s="14"/>
+    </row>
+    <row r="374">
+      <c r="A374" s="14"/>
+      <c r="B374" s="14"/>
+      <c r="C374" s="14"/>
+    </row>
+    <row r="375">
+      <c r="A375" s="14"/>
+      <c r="B375" s="14"/>
+      <c r="C375" s="14"/>
+    </row>
+    <row r="376">
+      <c r="A376" s="14"/>
+      <c r="B376" s="14"/>
+      <c r="C376" s="14"/>
+    </row>
+    <row r="377">
+      <c r="A377" s="14"/>
+      <c r="B377" s="14"/>
+      <c r="C377" s="14"/>
+    </row>
+    <row r="378">
+      <c r="A378" s="14"/>
+      <c r="B378" s="14"/>
+      <c r="C378" s="14"/>
+    </row>
+    <row r="379">
+      <c r="A379" s="14"/>
+      <c r="B379" s="14"/>
+      <c r="C379" s="14"/>
+    </row>
+    <row r="380">
+      <c r="A380" s="14"/>
+      <c r="B380" s="14"/>
+      <c r="C380" s="14"/>
+    </row>
+    <row r="381">
+      <c r="A381" s="14"/>
+      <c r="B381" s="14"/>
+      <c r="C381" s="14"/>
+    </row>
+    <row r="382">
+      <c r="A382" s="14"/>
+      <c r="B382" s="14"/>
+      <c r="C382" s="14"/>
+    </row>
+    <row r="383">
+      <c r="A383" s="14"/>
+      <c r="B383" s="14"/>
+      <c r="C383" s="14"/>
+    </row>
+    <row r="384">
+      <c r="A384" s="14"/>
+      <c r="B384" s="14"/>
+      <c r="C384" s="14"/>
+    </row>
+    <row r="385">
+      <c r="A385" s="14"/>
+      <c r="B385" s="14"/>
+      <c r="C385" s="14"/>
+    </row>
+    <row r="386">
+      <c r="A386" s="14"/>
+      <c r="B386" s="14"/>
+      <c r="C386" s="14"/>
+    </row>
+    <row r="387">
+      <c r="A387" s="14"/>
+      <c r="B387" s="14"/>
+      <c r="C387" s="14"/>
+    </row>
+    <row r="388">
+      <c r="A388" s="14"/>
+      <c r="B388" s="14"/>
+      <c r="C388" s="14"/>
+    </row>
+    <row r="389">
+      <c r="A389" s="14"/>
+      <c r="B389" s="14"/>
+      <c r="C389" s="14"/>
+    </row>
+    <row r="390">
+      <c r="A390" s="14"/>
+      <c r="B390" s="14"/>
+      <c r="C390" s="14"/>
+    </row>
+    <row r="391">
+      <c r="A391" s="14"/>
+      <c r="B391" s="14"/>
+      <c r="C391" s="14"/>
+    </row>
+    <row r="392">
+      <c r="A392" s="14"/>
+      <c r="B392" s="14"/>
+      <c r="C392" s="14"/>
+    </row>
+    <row r="393">
+      <c r="A393" s="14"/>
+      <c r="B393" s="14"/>
+      <c r="C393" s="14"/>
+    </row>
+    <row r="394">
+      <c r="A394" s="14"/>
+      <c r="B394" s="14"/>
+      <c r="C394" s="14"/>
+    </row>
+    <row r="395">
+      <c r="A395" s="14"/>
+      <c r="B395" s="14"/>
+      <c r="C395" s="14"/>
+    </row>
+    <row r="396">
+      <c r="A396" s="14"/>
+      <c r="B396" s="14"/>
+      <c r="C396" s="14"/>
+    </row>
+    <row r="397">
+      <c r="A397" s="14"/>
+      <c r="B397" s="14"/>
+      <c r="C397" s="14"/>
+    </row>
+    <row r="398">
+      <c r="A398" s="14"/>
+      <c r="B398" s="14"/>
+      <c r="C398" s="14"/>
+    </row>
+    <row r="399">
+      <c r="A399" s="14"/>
+      <c r="B399" s="14"/>
+      <c r="C399" s="14"/>
+    </row>
+    <row r="400">
+      <c r="A400" s="14"/>
+      <c r="B400" s="14"/>
+      <c r="C400" s="14"/>
+    </row>
+    <row r="401">
+      <c r="A401" s="14"/>
+      <c r="B401" s="14"/>
+      <c r="C401" s="14"/>
+    </row>
+    <row r="402">
+      <c r="A402" s="14"/>
+      <c r="B402" s="14"/>
+      <c r="C402" s="14"/>
+    </row>
+    <row r="403">
+      <c r="A403" s="14"/>
+      <c r="B403" s="14"/>
+      <c r="C403" s="14"/>
+    </row>
+    <row r="404">
+      <c r="A404" s="14"/>
+      <c r="B404" s="14"/>
+      <c r="C404" s="14"/>
+    </row>
+    <row r="405">
+      <c r="A405" s="14"/>
+      <c r="B405" s="14"/>
+      <c r="C405" s="14"/>
+    </row>
+    <row r="406">
+      <c r="A406" s="14"/>
+      <c r="B406" s="14"/>
+      <c r="C406" s="14"/>
+    </row>
+    <row r="407">
+      <c r="A407" s="14"/>
+      <c r="B407" s="14"/>
+      <c r="C407" s="14"/>
+    </row>
+    <row r="408">
+      <c r="A408" s="14"/>
+      <c r="B408" s="14"/>
+      <c r="C408" s="14"/>
+    </row>
+    <row r="409">
+      <c r="A409" s="14"/>
+      <c r="B409" s="14"/>
+      <c r="C409" s="14"/>
+    </row>
+    <row r="410">
+      <c r="A410" s="14"/>
+      <c r="B410" s="14"/>
+      <c r="C410" s="14"/>
+    </row>
+    <row r="411">
+      <c r="A411" s="14"/>
+      <c r="B411" s="14"/>
+      <c r="C411" s="14"/>
+    </row>
+    <row r="412">
+      <c r="A412" s="14"/>
+      <c r="B412" s="14"/>
+      <c r="C412" s="14"/>
+    </row>
+    <row r="413">
+      <c r="A413" s="14"/>
+      <c r="B413" s="14"/>
+      <c r="C413" s="14"/>
+    </row>
+    <row r="414">
+      <c r="A414" s="14"/>
+      <c r="B414" s="14"/>
+      <c r="C414" s="14"/>
+    </row>
+    <row r="415">
+      <c r="A415" s="14"/>
+      <c r="B415" s="14"/>
+      <c r="C415" s="14"/>
+    </row>
+    <row r="416">
+      <c r="A416" s="14"/>
+      <c r="B416" s="14"/>
+      <c r="C416" s="14"/>
+    </row>
+    <row r="417">
+      <c r="A417" s="14"/>
+      <c r="B417" s="14"/>
+      <c r="C417" s="14"/>
+    </row>
+    <row r="418">
+      <c r="A418" s="14"/>
+      <c r="B418" s="14"/>
+      <c r="C418" s="14"/>
+    </row>
+    <row r="419">
+      <c r="A419" s="14"/>
+      <c r="B419" s="14"/>
+      <c r="C419" s="14"/>
+    </row>
+    <row r="420">
+      <c r="A420" s="14"/>
+      <c r="B420" s="14"/>
+      <c r="C420" s="14"/>
+    </row>
+    <row r="421">
+      <c r="A421" s="14"/>
+      <c r="B421" s="14"/>
+      <c r="C421" s="14"/>
+    </row>
+    <row r="422">
+      <c r="A422" s="14"/>
+      <c r="B422" s="14"/>
+      <c r="C422" s="14"/>
+    </row>
+    <row r="423">
+      <c r="A423" s="14"/>
+      <c r="B423" s="14"/>
+      <c r="C423" s="14"/>
+    </row>
+    <row r="424">
+      <c r="A424" s="14"/>
+      <c r="B424" s="14"/>
+      <c r="C424" s="14"/>
+    </row>
+    <row r="425">
+      <c r="A425" s="14"/>
+      <c r="B425" s="14"/>
+      <c r="C425" s="14"/>
+    </row>
+    <row r="426">
+      <c r="A426" s="14"/>
+      <c r="B426" s="14"/>
+      <c r="C426" s="14"/>
+    </row>
+    <row r="427">
+      <c r="A427" s="14"/>
+      <c r="B427" s="14"/>
+      <c r="C427" s="14"/>
+    </row>
+    <row r="428">
+      <c r="A428" s="14"/>
+      <c r="B428" s="14"/>
+      <c r="C428" s="14"/>
+    </row>
+    <row r="429">
+      <c r="A429" s="14"/>
+      <c r="B429" s="14"/>
+      <c r="C429" s="14"/>
+    </row>
+    <row r="430">
+      <c r="A430" s="14"/>
+      <c r="B430" s="14"/>
+      <c r="C430" s="14"/>
+    </row>
+    <row r="431">
+      <c r="A431" s="14"/>
+      <c r="B431" s="14"/>
+      <c r="C431" s="14"/>
+    </row>
+    <row r="432">
+      <c r="A432" s="14"/>
+      <c r="B432" s="14"/>
+      <c r="C432" s="14"/>
+    </row>
+    <row r="433">
+      <c r="A433" s="14"/>
+      <c r="B433" s="14"/>
+      <c r="C433" s="14"/>
+    </row>
+    <row r="434">
+      <c r="A434" s="14"/>
+      <c r="B434" s="14"/>
+      <c r="C434" s="14"/>
+    </row>
+    <row r="435">
+      <c r="A435" s="14"/>
+      <c r="B435" s="14"/>
+      <c r="C435" s="14"/>
+    </row>
+    <row r="436">
+      <c r="A436" s="14"/>
+      <c r="B436" s="14"/>
+      <c r="C436" s="14"/>
+    </row>
+    <row r="437">
+      <c r="A437" s="14"/>
+      <c r="B437" s="14"/>
+      <c r="C437" s="14"/>
+    </row>
+    <row r="438">
+      <c r="A438" s="14"/>
+      <c r="B438" s="14"/>
+      <c r="C438" s="14"/>
+    </row>
+    <row r="439">
+      <c r="A439" s="14"/>
+      <c r="B439" s="14"/>
+      <c r="C439" s="14"/>
+    </row>
+    <row r="440">
+      <c r="A440" s="14"/>
+      <c r="B440" s="14"/>
+      <c r="C440" s="14"/>
+    </row>
+    <row r="441">
+      <c r="A441" s="14"/>
+      <c r="B441" s="14"/>
+      <c r="C441" s="14"/>
+    </row>
+    <row r="442">
+      <c r="A442" s="14"/>
+      <c r="B442" s="14"/>
+      <c r="C442" s="14"/>
+    </row>
+    <row r="443">
+      <c r="A443" s="14"/>
+      <c r="B443" s="14"/>
+      <c r="C443" s="14"/>
+    </row>
+    <row r="444">
+      <c r="A444" s="14"/>
+      <c r="B444" s="14"/>
+      <c r="C444" s="14"/>
+    </row>
+    <row r="445">
+      <c r="A445" s="14"/>
+      <c r="B445" s="14"/>
+      <c r="C445" s="14"/>
+    </row>
+    <row r="446">
+      <c r="A446" s="14"/>
+      <c r="B446" s="14"/>
+      <c r="C446" s="14"/>
+    </row>
+    <row r="447">
+      <c r="A447" s="14"/>
+      <c r="B447" s="14"/>
+      <c r="C447" s="14"/>
+    </row>
+    <row r="448">
+      <c r="A448" s="14"/>
+      <c r="B448" s="14"/>
+      <c r="C448" s="14"/>
+    </row>
+    <row r="449">
+      <c r="A449" s="14"/>
+      <c r="B449" s="14"/>
+      <c r="C449" s="14"/>
+    </row>
+    <row r="450">
+      <c r="A450" s="14"/>
+      <c r="B450" s="14"/>
+      <c r="C450" s="14"/>
+    </row>
+    <row r="451">
+      <c r="A451" s="14"/>
+      <c r="B451" s="14"/>
+      <c r="C451" s="14"/>
+    </row>
+    <row r="452">
+      <c r="A452" s="14"/>
+      <c r="B452" s="14"/>
+      <c r="C452" s="14"/>
+    </row>
+    <row r="453">
+      <c r="A453" s="14"/>
+      <c r="B453" s="14"/>
+      <c r="C453" s="14"/>
+    </row>
+    <row r="454">
+      <c r="A454" s="14"/>
+      <c r="B454" s="14"/>
+      <c r="C454" s="14"/>
+    </row>
+    <row r="455">
+      <c r="A455" s="14"/>
+      <c r="B455" s="14"/>
+      <c r="C455" s="14"/>
+    </row>
+    <row r="456">
+      <c r="A456" s="14"/>
+      <c r="B456" s="14"/>
+      <c r="C456" s="14"/>
+    </row>
+    <row r="457">
+      <c r="A457" s="14"/>
+      <c r="B457" s="14"/>
+      <c r="C457" s="14"/>
+    </row>
+    <row r="458">
+      <c r="A458" s="14"/>
+      <c r="B458" s="14"/>
+      <c r="C458" s="14"/>
+    </row>
+    <row r="459">
+      <c r="A459" s="14"/>
+      <c r="B459" s="14"/>
+      <c r="C459" s="14"/>
+    </row>
+    <row r="460">
+      <c r="A460" s="14"/>
+      <c r="B460" s="14"/>
+      <c r="C460" s="14"/>
+    </row>
+    <row r="461">
+      <c r="A461" s="14"/>
+      <c r="B461" s="14"/>
+      <c r="C461" s="14"/>
+    </row>
+    <row r="462">
+      <c r="A462" s="14"/>
+      <c r="B462" s="14"/>
+      <c r="C462" s="14"/>
+    </row>
+    <row r="463">
+      <c r="A463" s="14"/>
+      <c r="B463" s="14"/>
+      <c r="C463" s="14"/>
+    </row>
+    <row r="464">
+      <c r="A464" s="14"/>
+      <c r="B464" s="14"/>
+      <c r="C464" s="14"/>
+    </row>
+    <row r="465">
+      <c r="A465" s="14"/>
+      <c r="B465" s="14"/>
+      <c r="C465" s="14"/>
+    </row>
+    <row r="466">
+      <c r="A466" s="14"/>
+      <c r="B466" s="14"/>
+      <c r="C466" s="14"/>
+    </row>
+    <row r="467">
+      <c r="A467" s="14"/>
+      <c r="B467" s="14"/>
+      <c r="C467" s="14"/>
+    </row>
+    <row r="468">
+      <c r="A468" s="14"/>
+      <c r="B468" s="14"/>
+      <c r="C468" s="14"/>
+    </row>
+    <row r="469">
+      <c r="A469" s="14"/>
+      <c r="B469" s="14"/>
+      <c r="C469" s="14"/>
+    </row>
+    <row r="470">
+      <c r="A470" s="14"/>
+      <c r="B470" s="14"/>
+      <c r="C470" s="14"/>
+    </row>
+    <row r="471">
+      <c r="A471" s="14"/>
+      <c r="B471" s="14"/>
+      <c r="C471" s="14"/>
+    </row>
+    <row r="472">
+      <c r="A472" s="14"/>
+      <c r="B472" s="14"/>
+      <c r="C472" s="14"/>
+    </row>
+    <row r="473">
+      <c r="A473" s="14"/>
+      <c r="B473" s="14"/>
+      <c r="C473" s="14"/>
+    </row>
+    <row r="474">
+      <c r="A474" s="14"/>
+      <c r="B474" s="14"/>
+      <c r="C474" s="14"/>
+    </row>
+    <row r="475">
+      <c r="A475" s="14"/>
+      <c r="B475" s="14"/>
+      <c r="C475" s="14"/>
+    </row>
+    <row r="476">
+      <c r="A476" s="14"/>
+      <c r="B476" s="14"/>
+      <c r="C476" s="14"/>
+    </row>
+    <row r="477">
+      <c r="A477" s="14"/>
+      <c r="B477" s="14"/>
+      <c r="C477" s="14"/>
+    </row>
+    <row r="478">
+      <c r="A478" s="14"/>
+      <c r="B478" s="14"/>
+      <c r="C478" s="14"/>
+    </row>
+    <row r="479">
+      <c r="A479" s="14"/>
+      <c r="B479" s="14"/>
+      <c r="C479" s="14"/>
+    </row>
+    <row r="480">
+      <c r="A480" s="14"/>
+      <c r="B480" s="14"/>
+      <c r="C480" s="14"/>
+    </row>
+    <row r="481">
+      <c r="A481" s="14"/>
+      <c r="B481" s="14"/>
+      <c r="C481" s="14"/>
+    </row>
+    <row r="482">
+      <c r="A482" s="14"/>
+      <c r="B482" s="14"/>
+      <c r="C482" s="14"/>
+    </row>
+    <row r="483">
+      <c r="A483" s="14"/>
+      <c r="B483" s="14"/>
+      <c r="C483" s="14"/>
+    </row>
+    <row r="484">
+      <c r="A484" s="14"/>
+      <c r="B484" s="14"/>
+      <c r="C484" s="14"/>
+    </row>
+    <row r="485">
+      <c r="A485" s="14"/>
+      <c r="B485" s="14"/>
+      <c r="C485" s="14"/>
+    </row>
+    <row r="486">
+      <c r="A486" s="14"/>
+      <c r="B486" s="14"/>
+      <c r="C486" s="14"/>
+    </row>
+    <row r="487">
+      <c r="A487" s="14"/>
+      <c r="B487" s="14"/>
+      <c r="C487" s="14"/>
+    </row>
+    <row r="488">
+      <c r="A488" s="14"/>
+      <c r="B488" s="14"/>
+      <c r="C488" s="14"/>
+    </row>
+    <row r="489">
+      <c r="A489" s="14"/>
+      <c r="B489" s="14"/>
+      <c r="C489" s="14"/>
+    </row>
+    <row r="490">
+      <c r="A490" s="14"/>
+      <c r="B490" s="14"/>
+      <c r="C490" s="14"/>
+    </row>
+    <row r="491">
+      <c r="A491" s="14"/>
+      <c r="B491" s="14"/>
+      <c r="C491" s="14"/>
+    </row>
+    <row r="492">
+      <c r="A492" s="14"/>
+      <c r="B492" s="14"/>
+      <c r="C492" s="14"/>
+    </row>
+    <row r="493">
+      <c r="A493" s="14"/>
+      <c r="B493" s="14"/>
+      <c r="C493" s="14"/>
+    </row>
+    <row r="494">
+      <c r="A494" s="14"/>
+      <c r="B494" s="14"/>
+      <c r="C494" s="14"/>
+    </row>
+    <row r="495">
+      <c r="A495" s="14"/>
+      <c r="B495" s="14"/>
+      <c r="C495" s="14"/>
+    </row>
+    <row r="496">
+      <c r="A496" s="14"/>
+      <c r="B496" s="14"/>
+      <c r="C496" s="14"/>
+    </row>
+    <row r="497">
+      <c r="A497" s="14"/>
+      <c r="B497" s="14"/>
+      <c r="C497" s="14"/>
+    </row>
+    <row r="498">
+      <c r="A498" s="14"/>
+      <c r="B498" s="14"/>
+      <c r="C498" s="14"/>
+    </row>
+    <row r="499">
+      <c r="A499" s="14"/>
+      <c r="B499" s="14"/>
+      <c r="C499" s="14"/>
+    </row>
+    <row r="500">
+      <c r="A500" s="14"/>
+      <c r="B500" s="14"/>
+      <c r="C500" s="14"/>
+    </row>
+    <row r="501">
+      <c r="A501" s="14"/>
+      <c r="B501" s="14"/>
+      <c r="C501" s="14"/>
+    </row>
+    <row r="502">
+      <c r="A502" s="14"/>
+      <c r="B502" s="14"/>
+      <c r="C502" s="14"/>
+    </row>
+    <row r="503">
+      <c r="A503" s="14"/>
+      <c r="B503" s="14"/>
+      <c r="C503" s="14"/>
+    </row>
+    <row r="504">
+      <c r="A504" s="14"/>
+      <c r="B504" s="14"/>
+      <c r="C504" s="14"/>
+    </row>
+    <row r="505">
+      <c r="A505" s="14"/>
+      <c r="B505" s="14"/>
+      <c r="C505" s="14"/>
+    </row>
+    <row r="506">
+      <c r="A506" s="14"/>
+      <c r="B506" s="14"/>
+      <c r="C506" s="14"/>
+    </row>
+    <row r="507">
+      <c r="A507" s="14"/>
+      <c r="B507" s="14"/>
+      <c r="C507" s="14"/>
+    </row>
+    <row r="508">
+      <c r="A508" s="14"/>
+      <c r="B508" s="14"/>
+      <c r="C508" s="14"/>
+    </row>
+    <row r="509">
+      <c r="A509" s="14"/>
+      <c r="B509" s="14"/>
+      <c r="C509" s="14"/>
+    </row>
+    <row r="510">
+      <c r="A510" s="14"/>
+      <c r="B510" s="14"/>
+      <c r="C510" s="14"/>
+    </row>
+    <row r="511">
+      <c r="A511" s="14"/>
+      <c r="B511" s="14"/>
+      <c r="C511" s="14"/>
+    </row>
+    <row r="512">
+      <c r="A512" s="14"/>
+      <c r="B512" s="14"/>
+      <c r="C512" s="14"/>
+    </row>
+    <row r="513">
+      <c r="A513" s="14"/>
+      <c r="B513" s="14"/>
+      <c r="C513" s="14"/>
+    </row>
+    <row r="514">
+      <c r="A514" s="14"/>
+      <c r="B514" s="14"/>
+      <c r="C514" s="14"/>
+    </row>
+    <row r="515">
+      <c r="A515" s="14"/>
+      <c r="B515" s="14"/>
+      <c r="C515" s="14"/>
+    </row>
+    <row r="516">
+      <c r="A516" s="14"/>
+      <c r="B516" s="14"/>
+      <c r="C516" s="14"/>
+    </row>
+    <row r="517">
+      <c r="A517" s="14"/>
+      <c r="B517" s="14"/>
+      <c r="C517" s="14"/>
+    </row>
+    <row r="518">
+      <c r="A518" s="14"/>
+      <c r="B518" s="14"/>
+      <c r="C518" s="14"/>
+    </row>
+    <row r="519">
+      <c r="A519" s="14"/>
+      <c r="B519" s="14"/>
+      <c r="C519" s="14"/>
+    </row>
+    <row r="520">
+      <c r="A520" s="14"/>
+      <c r="B520" s="14"/>
+      <c r="C520" s="14"/>
+    </row>
+    <row r="521">
+      <c r="A521" s="14"/>
+      <c r="B521" s="14"/>
+      <c r="C521" s="14"/>
+    </row>
+    <row r="522">
+      <c r="A522" s="14"/>
+      <c r="B522" s="14"/>
+      <c r="C522" s="14"/>
+    </row>
+    <row r="523">
+      <c r="A523" s="14"/>
+      <c r="B523" s="14"/>
+      <c r="C523" s="14"/>
+    </row>
+    <row r="524">
+      <c r="A524" s="14"/>
+      <c r="B524" s="14"/>
+      <c r="C524" s="14"/>
+    </row>
+    <row r="525">
+      <c r="A525" s="14"/>
+      <c r="B525" s="14"/>
+      <c r="C525" s="14"/>
+    </row>
+    <row r="526">
+      <c r="A526" s="14"/>
+      <c r="B526" s="14"/>
+      <c r="C526" s="14"/>
+    </row>
+    <row r="527">
+      <c r="A527" s="14"/>
+      <c r="B527" s="14"/>
+      <c r="C527" s="14"/>
+    </row>
+    <row r="528">
+      <c r="A528" s="14"/>
+      <c r="B528" s="14"/>
+      <c r="C528" s="14"/>
+    </row>
+    <row r="529">
+      <c r="A529" s="14"/>
+      <c r="B529" s="14"/>
+      <c r="C529" s="14"/>
+    </row>
+    <row r="530">
+      <c r="A530" s="14"/>
+      <c r="B530" s="14"/>
+      <c r="C530" s="14"/>
+    </row>
+    <row r="531">
+      <c r="A531" s="14"/>
+      <c r="B531" s="14"/>
+      <c r="C531" s="14"/>
+    </row>
+    <row r="532">
+      <c r="A532" s="14"/>
+      <c r="B532" s="14"/>
+      <c r="C532" s="14"/>
+    </row>
+    <row r="533">
+      <c r="A533" s="14"/>
+      <c r="B533" s="14"/>
+      <c r="C533" s="14"/>
+    </row>
+    <row r="534">
+      <c r="A534" s="14"/>
+      <c r="B534" s="14"/>
+      <c r="C534" s="14"/>
+    </row>
+    <row r="535">
+      <c r="A535" s="14"/>
+      <c r="B535" s="14"/>
+      <c r="C535" s="14"/>
+    </row>
+    <row r="536">
+      <c r="A536" s="14"/>
+      <c r="B536" s="14"/>
+      <c r="C536" s="14"/>
+    </row>
+    <row r="537">
+      <c r="A537" s="14"/>
+      <c r="B537" s="14"/>
+      <c r="C537" s="14"/>
+    </row>
+    <row r="538">
+      <c r="A538" s="14"/>
+      <c r="B538" s="14"/>
+      <c r="C538" s="14"/>
+    </row>
+    <row r="539">
+      <c r="A539" s="14"/>
+      <c r="B539" s="14"/>
+      <c r="C539" s="14"/>
+    </row>
+    <row r="540">
+      <c r="A540" s="14"/>
+      <c r="B540" s="14"/>
+      <c r="C540" s="14"/>
+    </row>
+    <row r="541">
+      <c r="A541" s="14"/>
+      <c r="B541" s="14"/>
+      <c r="C541" s="14"/>
+    </row>
+    <row r="542">
+      <c r="A542" s="14"/>
+      <c r="B542" s="14"/>
+      <c r="C542" s="14"/>
+    </row>
+    <row r="543">
+      <c r="A543" s="14"/>
+      <c r="B543" s="14"/>
+      <c r="C543" s="14"/>
+    </row>
+    <row r="544">
+      <c r="A544" s="14"/>
+      <c r="B544" s="14"/>
+      <c r="C544" s="14"/>
+    </row>
+    <row r="545">
+      <c r="A545" s="14"/>
+      <c r="B545" s="14"/>
+      <c r="C545" s="14"/>
+    </row>
+    <row r="546">
+      <c r="A546" s="14"/>
+      <c r="B546" s="14"/>
+      <c r="C546" s="14"/>
+    </row>
+    <row r="547">
+      <c r="A547" s="14"/>
+      <c r="B547" s="14"/>
+      <c r="C547" s="14"/>
+    </row>
+    <row r="548">
+      <c r="A548" s="14"/>
+      <c r="B548" s="14"/>
+      <c r="C548" s="14"/>
+    </row>
+    <row r="549">
+      <c r="A549" s="14"/>
+      <c r="B549" s="14"/>
+      <c r="C549" s="14"/>
+    </row>
+    <row r="550">
+      <c r="A550" s="14"/>
+      <c r="B550" s="14"/>
+      <c r="C550" s="14"/>
+    </row>
+    <row r="551">
+      <c r="A551" s="14"/>
+      <c r="B551" s="14"/>
+      <c r="C551" s="14"/>
+    </row>
+    <row r="552">
+      <c r="A552" s="14"/>
+      <c r="B552" s="14"/>
+      <c r="C552" s="14"/>
+    </row>
+    <row r="553">
+      <c r="A553" s="14"/>
+      <c r="B553" s="14"/>
+      <c r="C553" s="14"/>
+    </row>
+    <row r="554">
+      <c r="A554" s="14"/>
+      <c r="B554" s="14"/>
+      <c r="C554" s="14"/>
+    </row>
+    <row r="555">
+      <c r="A555" s="14"/>
+      <c r="B555" s="14"/>
+      <c r="C555" s="14"/>
+    </row>
+    <row r="556">
+      <c r="A556" s="14"/>
+      <c r="B556" s="14"/>
+      <c r="C556" s="14"/>
+    </row>
+    <row r="557">
+      <c r="A557" s="14"/>
+      <c r="B557" s="14"/>
+      <c r="C557" s="14"/>
+    </row>
+    <row r="558">
+      <c r="A558" s="14"/>
+      <c r="B558" s="14"/>
+      <c r="C558" s="14"/>
+    </row>
+    <row r="559">
+      <c r="A559" s="14"/>
+      <c r="B559" s="14"/>
+      <c r="C559" s="14"/>
+    </row>
+    <row r="560">
+      <c r="A560" s="14"/>
+      <c r="B560" s="14"/>
+      <c r="C560" s="14"/>
+    </row>
+    <row r="561">
+      <c r="A561" s="14"/>
+      <c r="B561" s="14"/>
+      <c r="C561" s="14"/>
+    </row>
+    <row r="562">
+      <c r="A562" s="14"/>
+      <c r="B562" s="14"/>
+      <c r="C562" s="14"/>
+    </row>
+    <row r="563">
+      <c r="A563" s="14"/>
+      <c r="B563" s="14"/>
+      <c r="C563" s="14"/>
+    </row>
+    <row r="564">
+      <c r="A564" s="14"/>
+      <c r="B564" s="14"/>
+      <c r="C564" s="14"/>
+    </row>
+    <row r="565">
+      <c r="A565" s="14"/>
+      <c r="B565" s="14"/>
+      <c r="C565" s="14"/>
+    </row>
+    <row r="566">
+      <c r="A566" s="14"/>
+      <c r="B566" s="14"/>
+      <c r="C566" s="14"/>
+    </row>
+    <row r="567">
+      <c r="A567" s="14"/>
+      <c r="B567" s="14"/>
+      <c r="C567" s="14"/>
+    </row>
+    <row r="568">
+      <c r="A568" s="14"/>
+      <c r="B568" s="14"/>
+      <c r="C568" s="14"/>
+    </row>
+    <row r="569">
+      <c r="A569" s="14"/>
+      <c r="B569" s="14"/>
+      <c r="C569" s="14"/>
+    </row>
+    <row r="570">
+      <c r="A570" s="14"/>
+      <c r="B570" s="14"/>
+      <c r="C570" s="14"/>
+    </row>
+    <row r="571">
+      <c r="A571" s="14"/>
+      <c r="B571" s="14"/>
+      <c r="C571" s="14"/>
+    </row>
+    <row r="572">
+      <c r="A572" s="14"/>
+      <c r="B572" s="14"/>
+      <c r="C572" s="14"/>
+    </row>
+    <row r="573">
+      <c r="A573" s="14"/>
+      <c r="B573" s="14"/>
+      <c r="C573" s="14"/>
+    </row>
+    <row r="574">
+      <c r="A574" s="14"/>
+      <c r="B574" s="14"/>
+      <c r="C574" s="14"/>
+    </row>
+    <row r="575">
+      <c r="A575" s="14"/>
+      <c r="B575" s="14"/>
+      <c r="C575" s="14"/>
+    </row>
+    <row r="576">
+      <c r="A576" s="14"/>
+      <c r="B576" s="14"/>
+      <c r="C576" s="14"/>
+    </row>
+    <row r="577">
+      <c r="A577" s="14"/>
+      <c r="B577" s="14"/>
+      <c r="C577" s="14"/>
+    </row>
+    <row r="578">
+      <c r="A578" s="14"/>
+      <c r="B578" s="14"/>
+      <c r="C578" s="14"/>
+    </row>
+    <row r="579">
+      <c r="A579" s="14"/>
+      <c r="B579" s="14"/>
+      <c r="C579" s="14"/>
+    </row>
+    <row r="580">
+      <c r="A580" s="14"/>
+      <c r="B580" s="14"/>
+      <c r="C580" s="14"/>
+    </row>
+    <row r="581">
+      <c r="A581" s="14"/>
+      <c r="B581" s="14"/>
+      <c r="C581" s="14"/>
+    </row>
+    <row r="582">
+      <c r="A582" s="14"/>
+      <c r="B582" s="14"/>
+      <c r="C582" s="14"/>
+    </row>
+    <row r="583">
+      <c r="A583" s="14"/>
+      <c r="B583" s="14"/>
+      <c r="C583" s="14"/>
+    </row>
+    <row r="584">
+      <c r="A584" s="14"/>
+      <c r="B584" s="14"/>
+      <c r="C584" s="14"/>
+    </row>
+    <row r="585">
+      <c r="A585" s="14"/>
+      <c r="B585" s="14"/>
+      <c r="C585" s="14"/>
+    </row>
+    <row r="586">
+      <c r="A586" s="14"/>
+      <c r="B586" s="14"/>
+      <c r="C586" s="14"/>
+    </row>
+    <row r="587">
+      <c r="A587" s="14"/>
+      <c r="B587" s="14"/>
+      <c r="C587" s="14"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="14"/>
+      <c r="B588" s="14"/>
+      <c r="C588" s="14"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="14"/>
+      <c r="B589" s="14"/>
+      <c r="C589" s="14"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="14"/>
+      <c r="B590" s="14"/>
+      <c r="C590" s="14"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="14"/>
+      <c r="B591" s="14"/>
+      <c r="C591" s="14"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="14"/>
+      <c r="B592" s="14"/>
+      <c r="C592" s="14"/>
+    </row>
+    <row r="593">
+      <c r="A593" s="14"/>
+      <c r="B593" s="14"/>
+      <c r="C593" s="14"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="14"/>
+      <c r="B594" s="14"/>
+      <c r="C594" s="14"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="14"/>
+      <c r="B595" s="14"/>
+      <c r="C595" s="14"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="14"/>
+      <c r="B596" s="14"/>
+      <c r="C596" s="14"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="14"/>
+      <c r="B597" s="14"/>
+      <c r="C597" s="14"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="14"/>
+      <c r="B598" s="14"/>
+      <c r="C598" s="14"/>
+    </row>
+    <row r="599">
+      <c r="A599" s="14"/>
+      <c r="B599" s="14"/>
+      <c r="C599" s="14"/>
+    </row>
+    <row r="600">
+      <c r="A600" s="14"/>
+      <c r="B600" s="14"/>
+      <c r="C600" s="14"/>
+    </row>
+    <row r="601">
+      <c r="A601" s="14"/>
+      <c r="B601" s="14"/>
+      <c r="C601" s="14"/>
+    </row>
+    <row r="602">
+      <c r="A602" s="14"/>
+      <c r="B602" s="14"/>
+      <c r="C602" s="14"/>
+    </row>
+    <row r="603">
+      <c r="A603" s="14"/>
+      <c r="B603" s="14"/>
+      <c r="C603" s="14"/>
+    </row>
+    <row r="604">
+      <c r="A604" s="14"/>
+      <c r="B604" s="14"/>
+      <c r="C604" s="14"/>
+    </row>
+    <row r="605">
+      <c r="A605" s="14"/>
+      <c r="B605" s="14"/>
+      <c r="C605" s="14"/>
+    </row>
+    <row r="606">
+      <c r="A606" s="14"/>
+      <c r="B606" s="14"/>
+      <c r="C606" s="14"/>
+    </row>
+    <row r="607">
+      <c r="A607" s="14"/>
+      <c r="B607" s="14"/>
+      <c r="C607" s="14"/>
+    </row>
+    <row r="608">
+      <c r="A608" s="14"/>
+      <c r="B608" s="14"/>
+      <c r="C608" s="14"/>
+    </row>
+    <row r="609">
+      <c r="A609" s="14"/>
+      <c r="B609" s="14"/>
+      <c r="C609" s="14"/>
+    </row>
+    <row r="610">
+      <c r="A610" s="14"/>
+      <c r="B610" s="14"/>
+      <c r="C610" s="14"/>
+    </row>
+    <row r="611">
+      <c r="A611" s="14"/>
+      <c r="B611" s="14"/>
+      <c r="C611" s="14"/>
+    </row>
+    <row r="612">
+      <c r="A612" s="14"/>
+      <c r="B612" s="14"/>
+      <c r="C612" s="14"/>
+    </row>
+    <row r="613">
+      <c r="A613" s="14"/>
+      <c r="B613" s="14"/>
+      <c r="C613" s="14"/>
+    </row>
+    <row r="614">
+      <c r="A614" s="14"/>
+      <c r="B614" s="14"/>
+      <c r="C614" s="14"/>
+    </row>
+    <row r="615">
+      <c r="A615" s="14"/>
+      <c r="B615" s="14"/>
+      <c r="C615" s="14"/>
+    </row>
+    <row r="616">
+      <c r="A616" s="14"/>
+      <c r="B616" s="14"/>
+      <c r="C616" s="14"/>
+    </row>
+    <row r="617">
+      <c r="A617" s="14"/>
+      <c r="B617" s="14"/>
+      <c r="C617" s="14"/>
+    </row>
+    <row r="618">
+      <c r="A618" s="14"/>
+      <c r="B618" s="14"/>
+      <c r="C618" s="14"/>
+    </row>
+    <row r="619">
+      <c r="A619" s="14"/>
+      <c r="B619" s="14"/>
+      <c r="C619" s="14"/>
+    </row>
+    <row r="620">
+      <c r="A620" s="14"/>
+      <c r="B620" s="14"/>
+      <c r="C620" s="14"/>
+    </row>
+    <row r="621">
+      <c r="A621" s="14"/>
+      <c r="B621" s="14"/>
+      <c r="C621" s="14"/>
+    </row>
+    <row r="622">
+      <c r="A622" s="14"/>
+      <c r="B622" s="14"/>
+      <c r="C622" s="14"/>
+    </row>
+    <row r="623">
+      <c r="A623" s="14"/>
+      <c r="B623" s="14"/>
+      <c r="C623" s="14"/>
+    </row>
+    <row r="624">
+      <c r="A624" s="14"/>
+      <c r="B624" s="14"/>
+      <c r="C624" s="14"/>
+    </row>
+    <row r="625">
+      <c r="A625" s="14"/>
+      <c r="B625" s="14"/>
+      <c r="C625" s="14"/>
+    </row>
+    <row r="626">
+      <c r="A626" s="14"/>
+      <c r="B626" s="14"/>
+      <c r="C626" s="14"/>
+    </row>
+    <row r="627">
+      <c r="A627" s="14"/>
+      <c r="B627" s="14"/>
+      <c r="C627" s="14"/>
+    </row>
+    <row r="628">
+      <c r="A628" s="14"/>
+      <c r="B628" s="14"/>
+      <c r="C628" s="14"/>
+    </row>
+    <row r="629">
+      <c r="A629" s="14"/>
+      <c r="B629" s="14"/>
+      <c r="C629" s="14"/>
+    </row>
+    <row r="630">
+      <c r="A630" s="14"/>
+      <c r="B630" s="14"/>
+      <c r="C630" s="14"/>
+    </row>
+    <row r="631">
+      <c r="A631" s="14"/>
+      <c r="B631" s="14"/>
+      <c r="C631" s="14"/>
+    </row>
+    <row r="632">
+      <c r="A632" s="14"/>
+      <c r="B632" s="14"/>
+      <c r="C632" s="14"/>
+    </row>
+    <row r="633">
+      <c r="A633" s="14"/>
+      <c r="B633" s="14"/>
+      <c r="C633" s="14"/>
+    </row>
+    <row r="634">
+      <c r="A634" s="14"/>
+      <c r="B634" s="14"/>
+      <c r="C634" s="14"/>
+    </row>
+    <row r="635">
+      <c r="A635" s="14"/>
+      <c r="B635" s="14"/>
+      <c r="C635" s="14"/>
+    </row>
+    <row r="636">
+      <c r="A636" s="14"/>
+      <c r="B636" s="14"/>
+      <c r="C636" s="14"/>
+    </row>
+    <row r="637">
+      <c r="A637" s="14"/>
+      <c r="B637" s="14"/>
+      <c r="C637" s="14"/>
+    </row>
+    <row r="638">
+      <c r="A638" s="14"/>
+      <c r="B638" s="14"/>
+      <c r="C638" s="14"/>
+    </row>
+    <row r="639">
+      <c r="A639" s="14"/>
+      <c r="B639" s="14"/>
+      <c r="C639" s="14"/>
+    </row>
+    <row r="640">
+      <c r="A640" s="14"/>
+      <c r="B640" s="14"/>
+      <c r="C640" s="14"/>
+    </row>
+    <row r="641">
+      <c r="A641" s="14"/>
+      <c r="B641" s="14"/>
+      <c r="C641" s="14"/>
+    </row>
+    <row r="642">
+      <c r="A642" s="14"/>
+      <c r="B642" s="14"/>
+      <c r="C642" s="14"/>
+    </row>
+    <row r="643">
+      <c r="A643" s="14"/>
+      <c r="B643" s="14"/>
+      <c r="C643" s="14"/>
+    </row>
+    <row r="644">
+      <c r="A644" s="14"/>
+      <c r="B644" s="14"/>
+      <c r="C644" s="14"/>
+    </row>
+    <row r="645">
+      <c r="A645" s="14"/>
+      <c r="B645" s="14"/>
+      <c r="C645" s="14"/>
+    </row>
+    <row r="646">
+      <c r="A646" s="14"/>
+      <c r="B646" s="14"/>
+      <c r="C646" s="14"/>
+    </row>
+    <row r="647">
+      <c r="A647" s="14"/>
+      <c r="B647" s="14"/>
+      <c r="C647" s="14"/>
+    </row>
+    <row r="648">
+      <c r="A648" s="14"/>
+      <c r="B648" s="14"/>
+      <c r="C648" s="14"/>
+    </row>
+    <row r="649">
+      <c r="A649" s="14"/>
+      <c r="B649" s="14"/>
+      <c r="C649" s="14"/>
+    </row>
+    <row r="650">
+      <c r="A650" s="14"/>
+      <c r="B650" s="14"/>
+      <c r="C650" s="14"/>
+    </row>
+    <row r="651">
+      <c r="A651" s="14"/>
+      <c r="B651" s="14"/>
+      <c r="C651" s="14"/>
+    </row>
+    <row r="652">
+      <c r="A652" s="14"/>
+      <c r="B652" s="14"/>
+      <c r="C652" s="14"/>
+    </row>
+    <row r="653">
+      <c r="A653" s="14"/>
+      <c r="B653" s="14"/>
+      <c r="C653" s="14"/>
+    </row>
+    <row r="654">
+      <c r="A654" s="14"/>
+      <c r="B654" s="14"/>
+      <c r="C654" s="14"/>
+    </row>
+    <row r="655">
+      <c r="A655" s="14"/>
+      <c r="B655" s="14"/>
+      <c r="C655" s="14"/>
+    </row>
+    <row r="656">
+      <c r="A656" s="14"/>
+      <c r="B656" s="14"/>
+      <c r="C656" s="14"/>
+    </row>
+    <row r="657">
+      <c r="A657" s="14"/>
+      <c r="B657" s="14"/>
+      <c r="C657" s="14"/>
+    </row>
+    <row r="658">
+      <c r="A658" s="14"/>
+      <c r="B658" s="14"/>
+      <c r="C658" s="14"/>
+    </row>
+    <row r="659">
+      <c r="A659" s="14"/>
+      <c r="B659" s="14"/>
+      <c r="C659" s="14"/>
+    </row>
+    <row r="660">
+      <c r="A660" s="14"/>
+      <c r="B660" s="14"/>
+      <c r="C660" s="14"/>
+    </row>
+    <row r="661">
+      <c r="A661" s="14"/>
+      <c r="B661" s="14"/>
+      <c r="C661" s="14"/>
+    </row>
+    <row r="662">
+      <c r="A662" s="14"/>
+      <c r="B662" s="14"/>
+      <c r="C662" s="14"/>
+    </row>
+    <row r="663">
+      <c r="A663" s="14"/>
+      <c r="B663" s="14"/>
+      <c r="C663" s="14"/>
+    </row>
+    <row r="664">
+      <c r="A664" s="14"/>
+      <c r="B664" s="14"/>
+      <c r="C664" s="14"/>
+    </row>
+    <row r="665">
+      <c r="A665" s="14"/>
+      <c r="B665" s="14"/>
+      <c r="C665" s="14"/>
+    </row>
+    <row r="666">
+      <c r="A666" s="14"/>
+      <c r="B666" s="14"/>
+      <c r="C666" s="14"/>
+    </row>
+    <row r="667">
+      <c r="A667" s="14"/>
+      <c r="B667" s="14"/>
+      <c r="C667" s="14"/>
+    </row>
+    <row r="668">
+      <c r="A668" s="14"/>
+      <c r="B668" s="14"/>
+      <c r="C668" s="14"/>
+    </row>
+    <row r="669">
+      <c r="A669" s="14"/>
+      <c r="B669" s="14"/>
+      <c r="C669" s="14"/>
+    </row>
+    <row r="670">
+      <c r="A670" s="14"/>
+      <c r="B670" s="14"/>
+      <c r="C670" s="14"/>
+    </row>
+    <row r="671">
+      <c r="A671" s="14"/>
+      <c r="B671" s="14"/>
+      <c r="C671" s="14"/>
+    </row>
+    <row r="672">
+      <c r="A672" s="14"/>
+      <c r="B672" s="14"/>
+      <c r="C672" s="14"/>
+    </row>
+    <row r="673">
+      <c r="A673" s="14"/>
+      <c r="B673" s="14"/>
+      <c r="C673" s="14"/>
+    </row>
+    <row r="674">
+      <c r="A674" s="14"/>
+      <c r="B674" s="14"/>
+      <c r="C674" s="14"/>
+    </row>
+    <row r="675">
+      <c r="A675" s="14"/>
+      <c r="B675" s="14"/>
+      <c r="C675" s="14"/>
+    </row>
+    <row r="676">
+      <c r="A676" s="14"/>
+      <c r="B676" s="14"/>
+      <c r="C676" s="14"/>
+    </row>
+    <row r="677">
+      <c r="A677" s="14"/>
+      <c r="B677" s="14"/>
+      <c r="C677" s="14"/>
+    </row>
+    <row r="678">
+      <c r="A678" s="14"/>
+      <c r="B678" s="14"/>
+      <c r="C678" s="14"/>
+    </row>
+    <row r="679">
+      <c r="A679" s="14"/>
+      <c r="B679" s="14"/>
+      <c r="C679" s="14"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="G2"/>
+    <hyperlink r:id="rId2" ref="G3"/>
+    <hyperlink r:id="rId3" ref="G4"/>
+    <hyperlink r:id="rId4" ref="G5"/>
+    <hyperlink r:id="rId5" ref="G6"/>
+    <hyperlink r:id="rId6" ref="G8"/>
+    <hyperlink r:id="rId7" ref="G9"/>
+    <hyperlink r:id="rId8" ref="G10"/>
+  </hyperlinks>
+  <drawing r:id="rId9"/>
+</worksheet>
 </file>
</xml_diff>